<commit_message>
data(tests): fix Georgia testing data cutoff #2278
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="856">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -183,7 +183,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2022/01/coronavirus-covid-19-at-a-glance-13-january-2022.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2022/01/coronavirus-covid-19-at-a-glance-19-january-2022.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -544,7 +544,7 @@
     <t xml:space="preserve">Cape Verde - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://covid19.cv/boletim-epidemiologico-de-16-de-janeiro-de-2022/</t>
+    <t xml:space="preserve">https://covid19.cv/boletim-epidemiologico-de-18-de-janeiro-de-2022/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Cape Verde</t>
@@ -1261,10 +1261,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://irangov.ir/detail/378263</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ministry of Health and Medical Education</t>
+    <t xml:space="preserve">http://irangov.ir/detail/378453</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -2435,13 +2432,13 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://sites.google.com/view/snuaric/data-service/covid-19/covid-19-data?authuser=0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Korea Disease Control and Prevention Agency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suspicious report testing + testing at temporary screening stations</t>
+    <t xml:space="preserve">https://sites.google.com/view/snuaric/data-service/covid-19/covid-19-data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korea Disease Control and prevention Agency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data made available by Asia Regional Information Center at Seoul National University</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Welfare</t>
@@ -3516,8 +3513,12 @@
       <c r="M6" t="n">
         <v>1.757</v>
       </c>
-      <c r="N6"/>
-      <c r="O6"/>
+      <c r="N6" t="n">
+        <v>0.0494</v>
+      </c>
+      <c r="O6" t="n">
+        <v>20.2</v>
+      </c>
       <c r="P6" t="s">
         <v>36</v>
       </c>
@@ -3539,7 +3540,7 @@
         <v>52</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>44574</v>
+        <v>44580</v>
       </c>
       <c r="D7" t="s">
         <v>53</v>
@@ -3549,31 +3550,31 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="H7" t="n">
-        <v>58069697</v>
+        <v>59362737</v>
       </c>
       <c r="I7" t="n">
-        <v>2251.792</v>
+        <v>2301.933</v>
       </c>
       <c r="J7" t="n">
-        <v>219303</v>
+        <v>205569</v>
       </c>
       <c r="K7" t="n">
-        <v>8.504</v>
+        <v>7.971</v>
       </c>
       <c r="L7" t="n">
-        <v>248994</v>
+        <v>216049</v>
       </c>
       <c r="M7" t="n">
-        <v>9.655</v>
+        <v>8.378</v>
       </c>
       <c r="N7" t="n">
-        <v>0.4386</v>
+        <v>0.4125</v>
       </c>
       <c r="O7" t="n">
-        <v>2.3</v>
+        <v>2.4</v>
       </c>
       <c r="P7" t="s">
         <v>54</v>
@@ -3626,8 +3627,12 @@
       <c r="M8" t="n">
         <v>77.184</v>
       </c>
-      <c r="N8"/>
-      <c r="O8"/>
+      <c r="N8" t="n">
+        <v>0.0223</v>
+      </c>
+      <c r="O8" t="n">
+        <v>44.8</v>
+      </c>
       <c r="P8" t="s">
         <v>60</v>
       </c>
@@ -3675,8 +3680,12 @@
       <c r="M9" t="n">
         <v>0.78</v>
       </c>
-      <c r="N9"/>
-      <c r="O9"/>
+      <c r="N9" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="O9" t="n">
+        <v>12.3</v>
+      </c>
       <c r="P9" t="s">
         <v>65</v>
       </c>
@@ -3781,8 +3790,12 @@
       <c r="M11" t="n">
         <v>14.343</v>
       </c>
-      <c r="N11"/>
-      <c r="O11"/>
+      <c r="N11" t="n">
+        <v>0.0937</v>
+      </c>
+      <c r="O11" t="n">
+        <v>10.7</v>
+      </c>
       <c r="P11" t="s">
         <v>76</v>
       </c>
@@ -3834,8 +3847,12 @@
       <c r="M12" t="n">
         <v>0.168</v>
       </c>
-      <c r="N12"/>
-      <c r="O12"/>
+      <c r="N12" t="n">
+        <v>0.1456</v>
+      </c>
+      <c r="O12" t="n">
+        <v>6.9</v>
+      </c>
       <c r="P12" t="s">
         <v>83</v>
       </c>
@@ -4095,8 +4112,12 @@
       <c r="M17" t="n">
         <v>37.152</v>
       </c>
-      <c r="N17"/>
-      <c r="O17"/>
+      <c r="N17" t="n">
+        <v>0.0013</v>
+      </c>
+      <c r="O17" t="n">
+        <v>759.6</v>
+      </c>
       <c r="P17" t="s">
         <v>36</v>
       </c>
@@ -4554,7 +4575,7 @@
         <v>161</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>44576</v>
+        <v>44578</v>
       </c>
       <c r="D26" t="s">
         <v>162</v>
@@ -4564,15 +4585,15 @@
       </c>
       <c r="F26"/>
       <c r="G26" t="n">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26" t="n">
-        <v>1031</v>
+        <v>1802</v>
       </c>
       <c r="K26" t="n">
-        <v>1.835</v>
+        <v>3.207</v>
       </c>
       <c r="L26"/>
       <c r="M26"/>
@@ -4629,8 +4650,12 @@
       <c r="M27" t="n">
         <v>4.263</v>
       </c>
-      <c r="N27"/>
-      <c r="O27"/>
+      <c r="N27" t="n">
+        <v>0.0908</v>
+      </c>
+      <c r="O27" t="n">
+        <v>11</v>
+      </c>
       <c r="P27" t="s">
         <v>170</v>
       </c>
@@ -4902,8 +4927,12 @@
       <c r="M32" t="n">
         <v>3.919</v>
       </c>
-      <c r="N32"/>
-      <c r="O32"/>
+      <c r="N32" t="n">
+        <v>0.4613</v>
+      </c>
+      <c r="O32" t="n">
+        <v>2.2</v>
+      </c>
       <c r="P32" t="s">
         <v>199</v>
       </c>
@@ -5293,8 +5322,12 @@
       <c r="M39" t="n">
         <v>0.726</v>
       </c>
-      <c r="N39"/>
-      <c r="O39"/>
+      <c r="N39" t="n">
+        <v>0.4732</v>
+      </c>
+      <c r="O39" t="n">
+        <v>2.1</v>
+      </c>
       <c r="P39" t="s">
         <v>240</v>
       </c>
@@ -5399,8 +5432,12 @@
       <c r="M41" t="n">
         <v>0.324</v>
       </c>
-      <c r="N41"/>
-      <c r="O41"/>
+      <c r="N41" t="n">
+        <v>0.1888</v>
+      </c>
+      <c r="O41" t="n">
+        <v>5.3</v>
+      </c>
       <c r="P41" t="s">
         <v>253</v>
       </c>
@@ -5532,7 +5569,7 @@
         <v>267</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44572</v>
+        <v>44575</v>
       </c>
       <c r="D44" t="s">
         <v>268</v>
@@ -5547,7 +5584,7 @@
       <c r="J44"/>
       <c r="K44"/>
       <c r="L44" t="n">
-        <v>7264795</v>
+        <v>6709590</v>
       </c>
       <c r="M44"/>
       <c r="N44"/>
@@ -5905,14 +5942,10 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>74</v>
-      </c>
-      <c r="H51" t="n">
-        <v>3219094</v>
-      </c>
-      <c r="I51" t="n">
-        <v>808.864</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="H51"/>
+      <c r="I51"/>
       <c r="J51" t="n">
         <v>29711</v>
       </c>
@@ -5925,8 +5958,12 @@
       <c r="M51" t="n">
         <v>13.531</v>
       </c>
-      <c r="N51"/>
-      <c r="O51"/>
+      <c r="N51" t="n">
+        <v>0.0969</v>
+      </c>
+      <c r="O51" t="n">
+        <v>10.3</v>
+      </c>
       <c r="P51" t="s">
         <v>309</v>
       </c>
@@ -6080,8 +6117,12 @@
       <c r="M54" t="n">
         <v>32.685</v>
       </c>
-      <c r="N54"/>
-      <c r="O54"/>
+      <c r="N54" t="n">
+        <v>0.0608</v>
+      </c>
+      <c r="O54" t="n">
+        <v>16.4</v>
+      </c>
       <c r="P54" t="s">
         <v>329</v>
       </c>
@@ -6286,8 +6327,12 @@
       <c r="M58" t="n">
         <v>2.545</v>
       </c>
-      <c r="N58"/>
-      <c r="O58"/>
+      <c r="N58" t="n">
+        <v>0.295</v>
+      </c>
+      <c r="O58" t="n">
+        <v>3.4</v>
+      </c>
       <c r="P58" t="s">
         <v>355</v>
       </c>
@@ -6394,8 +6439,12 @@
       <c r="M60" t="n">
         <v>1.249</v>
       </c>
-      <c r="N60"/>
-      <c r="O60"/>
+      <c r="N60" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="O60" t="n">
+        <v>7</v>
+      </c>
       <c r="P60" t="s">
         <v>367</v>
       </c>
@@ -6447,8 +6496,12 @@
       <c r="M61" t="n">
         <v>0.691</v>
       </c>
-      <c r="N61"/>
-      <c r="O61"/>
+      <c r="N61" t="n">
+        <v>0.0043</v>
+      </c>
+      <c r="O61" t="n">
+        <v>231.7</v>
+      </c>
       <c r="P61" t="s">
         <v>373</v>
       </c>
@@ -6470,7 +6523,7 @@
         <v>377</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44578</v>
+        <v>44580</v>
       </c>
       <c r="D62" t="s">
         <v>378</v>
@@ -6480,56 +6533,60 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="H62" t="n">
-        <v>43499337</v>
+        <v>43680828</v>
       </c>
       <c r="I62" t="n">
-        <v>511.584</v>
+        <v>513.718</v>
       </c>
       <c r="J62" t="n">
-        <v>89216</v>
+        <v>91257</v>
       </c>
       <c r="K62" t="n">
-        <v>1.049</v>
+        <v>1.073</v>
       </c>
       <c r="L62" t="n">
-        <v>84462</v>
+        <v>87275</v>
       </c>
       <c r="M62" t="n">
-        <v>0.993</v>
-      </c>
-      <c r="N62"/>
-      <c r="O62"/>
+        <v>1.026</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="O62" t="n">
+        <v>31.3</v>
+      </c>
       <c r="P62" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q62" t="s">
         <v>380</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>381</v>
       </c>
       <c r="R62" t="s">
         <v>44</v>
       </c>
       <c r="S62" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
+        <v>382</v>
+      </c>
+      <c r="B63" t="s">
         <v>383</v>
-      </c>
-      <c r="B63" t="s">
-        <v>384</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>44574</v>
       </c>
       <c r="D63" t="s">
+        <v>384</v>
+      </c>
+      <c r="E63" t="s">
         <v>385</v>
-      </c>
-      <c r="E63" t="s">
-        <v>386</v>
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
@@ -6556,33 +6613,33 @@
         <v>10.8</v>
       </c>
       <c r="P63" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q63" t="s">
         <v>387</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>388</v>
       </c>
       <c r="R63" t="s">
         <v>114</v>
       </c>
       <c r="S63" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>389</v>
+      </c>
+      <c r="B64" t="s">
         <v>390</v>
-      </c>
-      <c r="B64" t="s">
-        <v>391</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D64" t="s">
+        <v>391</v>
+      </c>
+      <c r="E64" t="s">
         <v>392</v>
-      </c>
-      <c r="E64" t="s">
-        <v>393</v>
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
@@ -6606,36 +6663,40 @@
       <c r="M64" t="n">
         <v>6.863</v>
       </c>
-      <c r="N64"/>
-      <c r="O64"/>
+      <c r="N64" t="n">
+        <v>0.5502</v>
+      </c>
+      <c r="O64" t="n">
+        <v>1.8</v>
+      </c>
       <c r="P64" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q64" t="s">
         <v>393</v>
-      </c>
-      <c r="Q64" t="s">
-        <v>394</v>
       </c>
       <c r="R64" t="s">
         <v>44</v>
       </c>
       <c r="S64" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
+        <v>395</v>
+      </c>
+      <c r="B65" t="s">
         <v>396</v>
-      </c>
-      <c r="B65" t="s">
-        <v>397</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>44576</v>
       </c>
       <c r="D65" t="s">
+        <v>397</v>
+      </c>
+      <c r="E65" t="s">
         <v>398</v>
-      </c>
-      <c r="E65" t="s">
-        <v>399</v>
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
@@ -6669,33 +6730,33 @@
         <v>36</v>
       </c>
       <c r="Q65" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R65" t="s">
         <v>44</v>
       </c>
       <c r="S65" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
+        <v>400</v>
+      </c>
+      <c r="B66" t="s">
         <v>401</v>
-      </c>
-      <c r="B66" t="s">
-        <v>402</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D66" t="s">
+        <v>402</v>
+      </c>
+      <c r="E66" t="s">
         <v>403</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>404</v>
-      </c>
-      <c r="F66" t="s">
-        <v>405</v>
       </c>
       <c r="G66" t="n">
         <v>693</v>
@@ -6718,36 +6779,40 @@
       <c r="M66" t="n">
         <v>17.906</v>
       </c>
-      <c r="N66"/>
-      <c r="O66"/>
+      <c r="N66" t="n">
+        <v>0.1633</v>
+      </c>
+      <c r="O66" t="n">
+        <v>6.1</v>
+      </c>
       <c r="P66" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q66" t="s">
         <v>406</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>407</v>
       </c>
       <c r="R66" t="s">
         <v>44</v>
       </c>
       <c r="S66" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
+        <v>408</v>
+      </c>
+      <c r="B67" t="s">
         <v>409</v>
-      </c>
-      <c r="B67" t="s">
-        <v>410</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>44569</v>
       </c>
       <c r="D67" t="s">
+        <v>410</v>
+      </c>
+      <c r="E67" t="s">
         <v>411</v>
-      </c>
-      <c r="E67" t="s">
-        <v>412</v>
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
@@ -6778,33 +6843,33 @@
         <v>3.2</v>
       </c>
       <c r="P67" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q67" t="s">
         <v>412</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>413</v>
       </c>
       <c r="R67" t="s">
         <v>114</v>
       </c>
       <c r="S67" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
+        <v>414</v>
+      </c>
+      <c r="B68" t="s">
         <v>415</v>
-      </c>
-      <c r="B68" t="s">
-        <v>416</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D68" t="s">
+        <v>416</v>
+      </c>
+      <c r="E68" t="s">
         <v>417</v>
-      </c>
-      <c r="E68" t="s">
-        <v>418</v>
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
@@ -6835,33 +6900,33 @@
         <v>6.1</v>
       </c>
       <c r="P68" t="s">
+        <v>417</v>
+      </c>
+      <c r="Q68" t="s">
         <v>418</v>
-      </c>
-      <c r="Q68" t="s">
-        <v>419</v>
       </c>
       <c r="R68" t="s">
         <v>31</v>
       </c>
       <c r="S68" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
+        <v>420</v>
+      </c>
+      <c r="B69" t="s">
         <v>421</v>
-      </c>
-      <c r="B69" t="s">
-        <v>422</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D69" t="s">
+        <v>422</v>
+      </c>
+      <c r="E69" t="s">
         <v>423</v>
-      </c>
-      <c r="E69" t="s">
-        <v>424</v>
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
@@ -6892,33 +6957,33 @@
         <v>11.5</v>
       </c>
       <c r="P69" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q69" t="s">
         <v>424</v>
-      </c>
-      <c r="Q69" t="s">
-        <v>425</v>
       </c>
       <c r="R69" t="s">
         <v>44</v>
       </c>
       <c r="S69" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
+        <v>426</v>
+      </c>
+      <c r="B70" t="s">
         <v>427</v>
-      </c>
-      <c r="B70" t="s">
-        <v>428</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>44355</v>
       </c>
       <c r="D70" t="s">
+        <v>428</v>
+      </c>
+      <c r="E70" t="s">
         <v>429</v>
-      </c>
-      <c r="E70" t="s">
-        <v>430</v>
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
@@ -6949,33 +7014,33 @@
         <v>33.4</v>
       </c>
       <c r="P70" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q70" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="R70" t="s">
         <v>44</v>
       </c>
       <c r="S70" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
+        <v>431</v>
+      </c>
+      <c r="B71" t="s">
         <v>432</v>
-      </c>
-      <c r="B71" t="s">
-        <v>433</v>
       </c>
       <c r="C71" s="1" t="n">
         <v>44547</v>
       </c>
       <c r="D71" t="s">
+        <v>433</v>
+      </c>
+      <c r="E71" t="s">
         <v>434</v>
-      </c>
-      <c r="E71" t="s">
-        <v>435</v>
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
@@ -7005,30 +7070,30 @@
         <v>36</v>
       </c>
       <c r="Q71" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="R71" t="s">
         <v>44</v>
       </c>
       <c r="S71" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
+        <v>436</v>
+      </c>
+      <c r="B72" t="s">
         <v>437</v>
-      </c>
-      <c r="B72" t="s">
-        <v>438</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D72" t="s">
+        <v>438</v>
+      </c>
+      <c r="E72" t="s">
         <v>439</v>
-      </c>
-      <c r="E72" t="s">
-        <v>440</v>
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
@@ -7059,33 +7124,33 @@
         <v>12.7</v>
       </c>
       <c r="P72" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="Q72" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="R72" t="s">
         <v>24</v>
       </c>
       <c r="S72" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
+        <v>442</v>
+      </c>
+      <c r="B73" t="s">
         <v>443</v>
-      </c>
-      <c r="B73" t="s">
-        <v>444</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D73" t="s">
+        <v>444</v>
+      </c>
+      <c r="E73" t="s">
         <v>445</v>
-      </c>
-      <c r="E73" t="s">
-        <v>446</v>
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
@@ -7109,36 +7174,40 @@
       <c r="M73" t="n">
         <v>7.957</v>
       </c>
-      <c r="N73"/>
-      <c r="O73"/>
+      <c r="N73" t="n">
+        <v>0.1364</v>
+      </c>
+      <c r="O73" t="n">
+        <v>7.3</v>
+      </c>
       <c r="P73" t="s">
+        <v>445</v>
+      </c>
+      <c r="Q73" t="s">
         <v>446</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>447</v>
       </c>
       <c r="R73" t="s">
         <v>44</v>
       </c>
       <c r="S73" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
+        <v>448</v>
+      </c>
+      <c r="B74" t="s">
         <v>449</v>
-      </c>
-      <c r="B74" t="s">
-        <v>450</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>44570</v>
       </c>
       <c r="D74" t="s">
+        <v>450</v>
+      </c>
+      <c r="E74" t="s">
         <v>451</v>
-      </c>
-      <c r="E74" t="s">
-        <v>452</v>
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
@@ -7165,36 +7234,36 @@
         <v>2.5</v>
       </c>
       <c r="P74" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="Q74" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="R74" t="s">
         <v>275</v>
       </c>
       <c r="S74" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
+        <v>453</v>
+      </c>
+      <c r="B75" t="s">
         <v>454</v>
-      </c>
-      <c r="B75" t="s">
-        <v>455</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D75" t="s">
+        <v>455</v>
+      </c>
+      <c r="E75" t="s">
         <v>456</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F75" t="s">
         <v>457</v>
-      </c>
-      <c r="F75" t="s">
-        <v>458</v>
       </c>
       <c r="G75" t="n">
         <v>689</v>
@@ -7217,36 +7286,40 @@
       <c r="M75" t="n">
         <v>7.813</v>
       </c>
-      <c r="N75"/>
-      <c r="O75"/>
+      <c r="N75" t="n">
+        <v>0.163</v>
+      </c>
+      <c r="O75" t="n">
+        <v>6.1</v>
+      </c>
       <c r="P75" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Q75" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="R75" t="s">
         <v>44</v>
       </c>
       <c r="S75" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
+        <v>459</v>
+      </c>
+      <c r="B76" t="s">
         <v>460</v>
-      </c>
-      <c r="B76" t="s">
-        <v>461</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>44370</v>
       </c>
       <c r="D76" t="s">
+        <v>461</v>
+      </c>
+      <c r="E76" t="s">
         <v>462</v>
-      </c>
-      <c r="E76" t="s">
-        <v>463</v>
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
@@ -7269,33 +7342,33 @@
       <c r="N76"/>
       <c r="O76"/>
       <c r="P76" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="Q76" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="R76" t="s">
         <v>24</v>
       </c>
       <c r="S76" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
+        <v>464</v>
+      </c>
+      <c r="B77" t="s">
         <v>465</v>
-      </c>
-      <c r="B77" t="s">
-        <v>466</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>44560</v>
       </c>
       <c r="D77" t="s">
+        <v>466</v>
+      </c>
+      <c r="E77" t="s">
         <v>467</v>
-      </c>
-      <c r="E77" t="s">
-        <v>468</v>
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
@@ -7314,33 +7387,33 @@
       <c r="N77"/>
       <c r="O77"/>
       <c r="P77" t="s">
+        <v>467</v>
+      </c>
+      <c r="Q77" t="s">
         <v>468</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>469</v>
       </c>
       <c r="R77" t="s">
         <v>114</v>
       </c>
       <c r="S77" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>470</v>
+      </c>
+      <c r="B78" t="s">
         <v>471</v>
-      </c>
-      <c r="B78" t="s">
-        <v>472</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>44571</v>
       </c>
       <c r="D78" t="s">
+        <v>472</v>
+      </c>
+      <c r="E78" t="s">
         <v>473</v>
-      </c>
-      <c r="E78" t="s">
-        <v>474</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
@@ -7371,33 +7444,33 @@
         <v>2.9</v>
       </c>
       <c r="P78" t="s">
+        <v>473</v>
+      </c>
+      <c r="Q78" t="s">
         <v>474</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>475</v>
       </c>
       <c r="R78" t="s">
         <v>44</v>
       </c>
       <c r="S78" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
+        <v>476</v>
+      </c>
+      <c r="B79" t="s">
         <v>477</v>
-      </c>
-      <c r="B79" t="s">
-        <v>478</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>44573</v>
       </c>
       <c r="D79" t="s">
+        <v>478</v>
+      </c>
+      <c r="E79" t="s">
         <v>479</v>
-      </c>
-      <c r="E79" t="s">
-        <v>480</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
@@ -7428,33 +7501,33 @@
         <v>5.4</v>
       </c>
       <c r="P79" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="Q79" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="R79" t="s">
         <v>44</v>
       </c>
       <c r="S79" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
+        <v>481</v>
+      </c>
+      <c r="B80" t="s">
         <v>482</v>
-      </c>
-      <c r="B80" t="s">
-        <v>483</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>44576</v>
       </c>
       <c r="D80" t="s">
+        <v>483</v>
+      </c>
+      <c r="E80" t="s">
         <v>484</v>
-      </c>
-      <c r="E80" t="s">
-        <v>485</v>
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
@@ -7478,36 +7551,40 @@
       <c r="M80" t="n">
         <v>8.426</v>
       </c>
-      <c r="N80"/>
-      <c r="O80"/>
+      <c r="N80" t="n">
+        <v>0.2974</v>
+      </c>
+      <c r="O80" t="n">
+        <v>3.4</v>
+      </c>
       <c r="P80" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q80" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="R80" t="s">
         <v>44</v>
       </c>
       <c r="S80" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
+        <v>486</v>
+      </c>
+      <c r="B81" t="s">
         <v>487</v>
-      </c>
-      <c r="B81" t="s">
-        <v>488</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>44575</v>
       </c>
       <c r="D81" t="s">
+        <v>488</v>
+      </c>
+      <c r="E81" t="s">
         <v>489</v>
-      </c>
-      <c r="E81" t="s">
-        <v>490</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
@@ -7534,33 +7611,33 @@
         <v>6.5</v>
       </c>
       <c r="P81" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q81" t="s">
         <v>490</v>
-      </c>
-      <c r="Q81" t="s">
-        <v>491</v>
       </c>
       <c r="R81" t="s">
         <v>44</v>
       </c>
       <c r="S81" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
+        <v>492</v>
+      </c>
+      <c r="B82" t="s">
         <v>493</v>
-      </c>
-      <c r="B82" t="s">
-        <v>494</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>44400</v>
       </c>
       <c r="D82" t="s">
+        <v>494</v>
+      </c>
+      <c r="E82" t="s">
         <v>495</v>
-      </c>
-      <c r="E82" t="s">
-        <v>496</v>
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
@@ -7587,36 +7664,36 @@
         <v>3.1</v>
       </c>
       <c r="P82" t="s">
+        <v>495</v>
+      </c>
+      <c r="Q82" t="s">
         <v>496</v>
-      </c>
-      <c r="Q82" t="s">
-        <v>497</v>
       </c>
       <c r="R82" t="s">
         <v>114</v>
       </c>
       <c r="S82" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
+        <v>498</v>
+      </c>
+      <c r="B83" t="s">
         <v>499</v>
-      </c>
-      <c r="B83" t="s">
-        <v>500</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>44576</v>
       </c>
       <c r="D83" t="s">
+        <v>500</v>
+      </c>
+      <c r="E83" t="s">
         <v>501</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F83" t="s">
         <v>502</v>
-      </c>
-      <c r="F83" t="s">
-        <v>503</v>
       </c>
       <c r="G83" t="n">
         <v>723</v>
@@ -7649,30 +7726,30 @@
         <v>36</v>
       </c>
       <c r="Q83" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="R83" t="s">
         <v>31</v>
       </c>
       <c r="S83" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
+        <v>505</v>
+      </c>
+      <c r="B84" t="s">
         <v>506</v>
-      </c>
-      <c r="B84" t="s">
-        <v>507</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D84" t="s">
+        <v>507</v>
+      </c>
+      <c r="E84" t="s">
         <v>508</v>
-      </c>
-      <c r="E84" t="s">
-        <v>509</v>
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
@@ -7696,36 +7773,40 @@
       <c r="M84" t="n">
         <v>11.729</v>
       </c>
-      <c r="N84"/>
-      <c r="O84"/>
+      <c r="N84" t="n">
+        <v>0.1455</v>
+      </c>
+      <c r="O84" t="n">
+        <v>6.9</v>
+      </c>
       <c r="P84" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q84" t="s">
         <v>509</v>
-      </c>
-      <c r="Q84" t="s">
-        <v>510</v>
       </c>
       <c r="R84" t="s">
         <v>114</v>
       </c>
       <c r="S84" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
+        <v>511</v>
+      </c>
+      <c r="B85" t="s">
         <v>512</v>
-      </c>
-      <c r="B85" t="s">
-        <v>513</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D85" t="s">
+        <v>513</v>
+      </c>
+      <c r="E85" t="s">
         <v>514</v>
-      </c>
-      <c r="E85" t="s">
-        <v>515</v>
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
@@ -7749,33 +7830,37 @@
       <c r="M85" t="n">
         <v>8.243</v>
       </c>
-      <c r="N85"/>
-      <c r="O85"/>
+      <c r="N85" t="n">
+        <v>0.1066</v>
+      </c>
+      <c r="O85" t="n">
+        <v>9.4</v>
+      </c>
       <c r="P85" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q85" t="s">
         <v>516</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>517</v>
       </c>
       <c r="R85" t="s">
         <v>44</v>
       </c>
       <c r="S85" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
+        <v>518</v>
+      </c>
+      <c r="B86" t="s">
         <v>519</v>
-      </c>
-      <c r="B86" t="s">
-        <v>520</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>44290</v>
       </c>
       <c r="D86" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E86" t="s">
         <v>36</v>
@@ -7801,33 +7886,33 @@
       <c r="N86"/>
       <c r="O86"/>
       <c r="P86" t="s">
+        <v>521</v>
+      </c>
+      <c r="Q86" t="s">
         <v>522</v>
-      </c>
-      <c r="Q86" t="s">
-        <v>523</v>
       </c>
       <c r="R86" t="s">
         <v>44</v>
       </c>
       <c r="S86" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
+        <v>524</v>
+      </c>
+      <c r="B87" t="s">
         <v>525</v>
-      </c>
-      <c r="B87" t="s">
-        <v>526</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>44576</v>
       </c>
       <c r="D87" t="s">
+        <v>526</v>
+      </c>
+      <c r="E87" t="s">
         <v>527</v>
-      </c>
-      <c r="E87" t="s">
-        <v>528</v>
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
@@ -7858,33 +7943,33 @@
         <v>1.6</v>
       </c>
       <c r="P87" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Q87" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="R87" t="s">
         <v>31</v>
       </c>
       <c r="S87" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
+        <v>530</v>
+      </c>
+      <c r="B88" t="s">
         <v>531</v>
-      </c>
-      <c r="B88" t="s">
-        <v>532</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>44512</v>
       </c>
       <c r="D88" t="s">
+        <v>532</v>
+      </c>
+      <c r="E88" t="s">
         <v>533</v>
-      </c>
-      <c r="E88" t="s">
-        <v>534</v>
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
@@ -7911,30 +7996,30 @@
         <v>7</v>
       </c>
       <c r="P88" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Q88" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="R88" t="s">
         <v>24</v>
       </c>
       <c r="S88" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
+        <v>535</v>
+      </c>
+      <c r="B89" t="s">
         <v>536</v>
-      </c>
-      <c r="B89" t="s">
-        <v>537</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D89" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E89" t="s">
         <v>36</v>
@@ -7957,36 +8042,40 @@
       <c r="M89" t="n">
         <v>5.492</v>
       </c>
-      <c r="N89"/>
-      <c r="O89"/>
+      <c r="N89" t="n">
+        <v>0.1173</v>
+      </c>
+      <c r="O89" t="n">
+        <v>8.5</v>
+      </c>
       <c r="P89" t="s">
         <v>36</v>
       </c>
       <c r="Q89" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="R89" t="s">
         <v>114</v>
       </c>
       <c r="S89" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
+        <v>540</v>
+      </c>
+      <c r="B90" t="s">
         <v>541</v>
-      </c>
-      <c r="B90" t="s">
-        <v>542</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D90" t="s">
+        <v>542</v>
+      </c>
+      <c r="E90" t="s">
         <v>543</v>
-      </c>
-      <c r="E90" t="s">
-        <v>544</v>
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
@@ -8017,33 +8106,33 @@
         <v>4.1</v>
       </c>
       <c r="P90" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q90" t="s">
         <v>544</v>
-      </c>
-      <c r="Q90" t="s">
-        <v>545</v>
       </c>
       <c r="R90" t="s">
         <v>31</v>
       </c>
       <c r="S90" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
+        <v>546</v>
+      </c>
+      <c r="B91" t="s">
         <v>547</v>
-      </c>
-      <c r="B91" t="s">
-        <v>548</v>
       </c>
       <c r="C91" s="1" t="n">
         <v>44558</v>
       </c>
       <c r="D91" t="s">
+        <v>548</v>
+      </c>
+      <c r="E91" t="s">
         <v>549</v>
-      </c>
-      <c r="E91" t="s">
-        <v>550</v>
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
@@ -8074,33 +8163,33 @@
         <v>2.5</v>
       </c>
       <c r="P91" t="s">
+        <v>549</v>
+      </c>
+      <c r="Q91" t="s">
         <v>550</v>
-      </c>
-      <c r="Q91" t="s">
-        <v>551</v>
       </c>
       <c r="R91" t="s">
         <v>78</v>
       </c>
       <c r="S91" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
+        <v>552</v>
+      </c>
+      <c r="B92" t="s">
         <v>553</v>
-      </c>
-      <c r="B92" t="s">
-        <v>554</v>
       </c>
       <c r="C92" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D92" t="s">
+        <v>554</v>
+      </c>
+      <c r="E92" t="s">
         <v>555</v>
-      </c>
-      <c r="E92" t="s">
-        <v>556</v>
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
@@ -8120,36 +8209,40 @@
       <c r="M92" t="n">
         <v>0.156</v>
       </c>
-      <c r="N92"/>
-      <c r="O92"/>
+      <c r="N92" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="O92" t="n">
+        <v>55.4</v>
+      </c>
       <c r="P92" t="s">
+        <v>555</v>
+      </c>
+      <c r="Q92" t="s">
         <v>556</v>
-      </c>
-      <c r="Q92" t="s">
-        <v>557</v>
       </c>
       <c r="R92" t="s">
         <v>114</v>
       </c>
       <c r="S92" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
+        <v>558</v>
+      </c>
+      <c r="B93" t="s">
         <v>559</v>
-      </c>
-      <c r="B93" t="s">
-        <v>560</v>
       </c>
       <c r="C93" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D93" t="s">
+        <v>560</v>
+      </c>
+      <c r="E93" t="s">
         <v>561</v>
-      </c>
-      <c r="E93" t="s">
-        <v>562</v>
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
@@ -8180,33 +8273,33 @@
         <v>6</v>
       </c>
       <c r="P93" t="s">
+        <v>562</v>
+      </c>
+      <c r="Q93" t="s">
         <v>563</v>
-      </c>
-      <c r="Q93" t="s">
-        <v>564</v>
       </c>
       <c r="R93" t="s">
         <v>114</v>
       </c>
       <c r="S93" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
+        <v>565</v>
+      </c>
+      <c r="B94" t="s">
         <v>566</v>
-      </c>
-      <c r="B94" t="s">
-        <v>567</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D94" t="s">
+        <v>567</v>
+      </c>
+      <c r="E94" t="s">
         <v>568</v>
-      </c>
-      <c r="E94" t="s">
-        <v>569</v>
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
@@ -8230,36 +8323,40 @@
       <c r="M94" t="n">
         <v>0.388</v>
       </c>
-      <c r="N94"/>
-      <c r="O94"/>
+      <c r="N94" t="n">
+        <v>0.3166</v>
+      </c>
+      <c r="O94" t="n">
+        <v>3.2</v>
+      </c>
       <c r="P94" t="s">
+        <v>568</v>
+      </c>
+      <c r="Q94" t="s">
         <v>569</v>
-      </c>
-      <c r="Q94" t="s">
-        <v>570</v>
       </c>
       <c r="R94" t="s">
         <v>44</v>
       </c>
       <c r="S94" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
+        <v>571</v>
+      </c>
+      <c r="B95" t="s">
         <v>572</v>
-      </c>
-      <c r="B95" t="s">
-        <v>573</v>
       </c>
       <c r="C95" s="1" t="n">
         <v>44576</v>
       </c>
       <c r="D95" t="s">
+        <v>573</v>
+      </c>
+      <c r="E95" t="s">
         <v>574</v>
-      </c>
-      <c r="E95" t="s">
-        <v>575</v>
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
@@ -8290,30 +8387,30 @@
         <v>3</v>
       </c>
       <c r="P95" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q95" t="s">
         <v>575</v>
-      </c>
-      <c r="Q95" t="s">
-        <v>576</v>
       </c>
       <c r="R95" t="s">
         <v>31</v>
       </c>
       <c r="S95" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
+        <v>577</v>
+      </c>
+      <c r="B96" t="s">
         <v>578</v>
-      </c>
-      <c r="B96" t="s">
-        <v>579</v>
       </c>
       <c r="C96" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D96" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E96" t="s">
         <v>36</v>
@@ -8336,36 +8433,40 @@
       <c r="M96" t="n">
         <v>2.902</v>
       </c>
-      <c r="N96"/>
-      <c r="O96"/>
+      <c r="N96" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="O96" t="n">
+        <v>251.3</v>
+      </c>
       <c r="P96" t="s">
+        <v>580</v>
+      </c>
+      <c r="Q96" t="s">
         <v>581</v>
-      </c>
-      <c r="Q96" t="s">
-        <v>582</v>
       </c>
       <c r="R96" t="s">
         <v>44</v>
       </c>
       <c r="S96" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
+        <v>583</v>
+      </c>
+      <c r="B97" t="s">
         <v>584</v>
-      </c>
-      <c r="B97" t="s">
-        <v>585</v>
       </c>
       <c r="C97" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D97" t="s">
+        <v>585</v>
+      </c>
+      <c r="E97" t="s">
         <v>586</v>
-      </c>
-      <c r="E97" t="s">
-        <v>587</v>
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
@@ -8392,30 +8493,30 @@
         <v>22.8</v>
       </c>
       <c r="P97" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="Q97" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="R97" t="s">
         <v>114</v>
       </c>
       <c r="S97" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
+        <v>588</v>
+      </c>
+      <c r="B98" t="s">
         <v>589</v>
-      </c>
-      <c r="B98" t="s">
-        <v>590</v>
       </c>
       <c r="C98" s="1" t="n">
         <v>44571</v>
       </c>
       <c r="D98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E98" t="s">
         <v>36</v>
@@ -8448,30 +8549,30 @@
         <v>36</v>
       </c>
       <c r="Q98" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="R98" t="s">
         <v>44</v>
       </c>
       <c r="S98" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
+        <v>593</v>
+      </c>
+      <c r="B99" t="s">
         <v>594</v>
-      </c>
-      <c r="B99" t="s">
-        <v>595</v>
       </c>
       <c r="C99" s="1" t="n">
         <v>44576</v>
       </c>
       <c r="D99" t="s">
+        <v>595</v>
+      </c>
+      <c r="E99" t="s">
         <v>596</v>
-      </c>
-      <c r="E99" t="s">
-        <v>597</v>
       </c>
       <c r="F99"/>
       <c r="G99" t="n">
@@ -8502,33 +8603,33 @@
         <v>2.8</v>
       </c>
       <c r="P99" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="Q99" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="R99" t="s">
         <v>31</v>
       </c>
       <c r="S99" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
+        <v>598</v>
+      </c>
+      <c r="B100" t="s">
         <v>599</v>
-      </c>
-      <c r="B100" t="s">
-        <v>600</v>
       </c>
       <c r="C100" s="1" t="n">
         <v>44048</v>
       </c>
       <c r="D100" t="s">
+        <v>600</v>
+      </c>
+      <c r="E100" t="s">
         <v>601</v>
-      </c>
-      <c r="E100" t="s">
-        <v>602</v>
       </c>
       <c r="F100"/>
       <c r="G100" t="n">
@@ -8547,83 +8648,83 @@
       <c r="N100"/>
       <c r="O100"/>
       <c r="P100" t="s">
+        <v>601</v>
+      </c>
+      <c r="Q100" t="s">
         <v>602</v>
-      </c>
-      <c r="Q100" t="s">
-        <v>603</v>
       </c>
       <c r="R100" t="s">
         <v>78</v>
       </c>
       <c r="S100" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
+        <v>604</v>
+      </c>
+      <c r="B101" t="s">
         <v>605</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" s="1" t="n">
+        <v>44581</v>
+      </c>
+      <c r="D101" t="s">
         <v>606</v>
       </c>
-      <c r="C101" s="1" t="n">
-        <v>44578</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>607</v>
-      </c>
-      <c r="E101" t="s">
-        <v>608</v>
       </c>
       <c r="F101"/>
       <c r="G101" t="n">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="H101" t="n">
-        <v>24186508</v>
+        <v>24356373</v>
       </c>
       <c r="I101" t="n">
-        <v>107.4</v>
+        <v>108.154</v>
       </c>
       <c r="J101" t="n">
-        <v>49799</v>
+        <v>58943</v>
       </c>
       <c r="K101" t="n">
-        <v>0.221</v>
+        <v>0.262</v>
       </c>
       <c r="L101" t="n">
-        <v>48419</v>
+        <v>53124</v>
       </c>
       <c r="M101" t="n">
-        <v>0.215</v>
+        <v>0.236</v>
       </c>
       <c r="N101"/>
       <c r="O101"/>
       <c r="P101" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q101" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="R101" t="s">
         <v>44</v>
       </c>
       <c r="S101" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
+        <v>609</v>
+      </c>
+      <c r="B102" t="s">
         <v>610</v>
-      </c>
-      <c r="B102" t="s">
-        <v>611</v>
       </c>
       <c r="C102" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D102" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E102" t="s">
         <v>36</v>
@@ -8646,36 +8747,40 @@
       <c r="M102" t="n">
         <v>1.049</v>
       </c>
-      <c r="N102"/>
-      <c r="O102"/>
+      <c r="N102" t="n">
+        <v>0.0891</v>
+      </c>
+      <c r="O102" t="n">
+        <v>11.2</v>
+      </c>
       <c r="P102" t="s">
+        <v>612</v>
+      </c>
+      <c r="Q102" t="s">
         <v>613</v>
-      </c>
-      <c r="Q102" t="s">
-        <v>614</v>
       </c>
       <c r="R102" t="s">
         <v>44</v>
       </c>
       <c r="S102" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
+        <v>615</v>
+      </c>
+      <c r="B103" t="s">
         <v>616</v>
-      </c>
-      <c r="B103" t="s">
-        <v>617</v>
       </c>
       <c r="C103" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D103" t="s">
+        <v>617</v>
+      </c>
+      <c r="E103" t="s">
         <v>618</v>
-      </c>
-      <c r="E103" t="s">
-        <v>619</v>
       </c>
       <c r="F103"/>
       <c r="G103" t="n">
@@ -8706,30 +8811,30 @@
         <v>3.1</v>
       </c>
       <c r="P103" t="s">
+        <v>618</v>
+      </c>
+      <c r="Q103" t="s">
         <v>619</v>
-      </c>
-      <c r="Q103" t="s">
-        <v>620</v>
       </c>
       <c r="R103" t="s">
         <v>44</v>
       </c>
       <c r="S103" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
+        <v>621</v>
+      </c>
+      <c r="B104" t="s">
         <v>622</v>
-      </c>
-      <c r="B104" t="s">
-        <v>623</v>
       </c>
       <c r="C104" s="1" t="n">
         <v>44304</v>
       </c>
       <c r="D104" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E104" t="s">
         <v>348</v>
@@ -8762,30 +8867,30 @@
         <v>348</v>
       </c>
       <c r="Q104" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="R104" t="s">
         <v>24</v>
       </c>
       <c r="S104" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
+        <v>626</v>
+      </c>
+      <c r="B105" t="s">
         <v>627</v>
-      </c>
-      <c r="B105" t="s">
-        <v>628</v>
       </c>
       <c r="C105" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D105" t="s">
+        <v>628</v>
+      </c>
+      <c r="E105" t="s">
         <v>629</v>
-      </c>
-      <c r="E105" t="s">
-        <v>630</v>
       </c>
       <c r="F105"/>
       <c r="G105" t="n">
@@ -8809,33 +8914,37 @@
       <c r="M105" t="n">
         <v>1.732</v>
       </c>
-      <c r="N105"/>
-      <c r="O105"/>
+      <c r="N105" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="O105" t="n">
+        <v>29.1</v>
+      </c>
       <c r="P105" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q105" t="s">
         <v>630</v>
-      </c>
-      <c r="Q105" t="s">
-        <v>631</v>
       </c>
       <c r="R105" t="s">
         <v>44</v>
       </c>
       <c r="S105" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
+        <v>632</v>
+      </c>
+      <c r="B106" t="s">
         <v>633</v>
-      </c>
-      <c r="B106" t="s">
-        <v>634</v>
       </c>
       <c r="C106" s="1" t="n">
         <v>44557</v>
       </c>
       <c r="D106" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E106" t="s">
         <v>182</v>
@@ -8872,30 +8981,30 @@
         <v>182</v>
       </c>
       <c r="Q106" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="R106" t="s">
         <v>44</v>
       </c>
       <c r="S106" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
+        <v>637</v>
+      </c>
+      <c r="B107" t="s">
         <v>638</v>
-      </c>
-      <c r="B107" t="s">
-        <v>639</v>
       </c>
       <c r="C107" s="1" t="n">
         <v>44570</v>
       </c>
       <c r="D107" t="s">
+        <v>639</v>
+      </c>
+      <c r="E107" t="s">
         <v>640</v>
-      </c>
-      <c r="E107" t="s">
-        <v>641</v>
       </c>
       <c r="F107"/>
       <c r="G107" t="n">
@@ -8929,30 +9038,30 @@
         <v>348</v>
       </c>
       <c r="Q107" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="R107" t="s">
         <v>31</v>
       </c>
       <c r="S107" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
+        <v>643</v>
+      </c>
+      <c r="B108" t="s">
         <v>644</v>
-      </c>
-      <c r="B108" t="s">
-        <v>645</v>
       </c>
       <c r="C108" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D108" t="s">
+        <v>645</v>
+      </c>
+      <c r="E108" t="s">
         <v>646</v>
-      </c>
-      <c r="E108" t="s">
-        <v>647</v>
       </c>
       <c r="F108"/>
       <c r="G108" t="n">
@@ -8976,36 +9085,40 @@
       <c r="M108" t="n">
         <v>2.238</v>
       </c>
-      <c r="N108"/>
-      <c r="O108"/>
+      <c r="N108" t="n">
+        <v>0.1731</v>
+      </c>
+      <c r="O108" t="n">
+        <v>5.8</v>
+      </c>
       <c r="P108" t="s">
+        <v>646</v>
+      </c>
+      <c r="Q108" t="s">
         <v>647</v>
-      </c>
-      <c r="Q108" t="s">
-        <v>648</v>
       </c>
       <c r="R108" t="s">
         <v>31</v>
       </c>
       <c r="S108" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B109" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C109" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D109" t="s">
+        <v>645</v>
+      </c>
+      <c r="E109" t="s">
         <v>646</v>
-      </c>
-      <c r="E109" t="s">
-        <v>647</v>
       </c>
       <c r="F109"/>
       <c r="G109" t="n">
@@ -9036,30 +9149,30 @@
         <v>6.2</v>
       </c>
       <c r="P109" t="s">
+        <v>646</v>
+      </c>
+      <c r="Q109" t="s">
         <v>647</v>
-      </c>
-      <c r="Q109" t="s">
-        <v>648</v>
       </c>
       <c r="R109" t="s">
         <v>114</v>
       </c>
       <c r="S109" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
+        <v>650</v>
+      </c>
+      <c r="B110" t="s">
         <v>651</v>
-      </c>
-      <c r="B110" t="s">
-        <v>652</v>
       </c>
       <c r="C110" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D110" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E110" t="s">
         <v>36</v>
@@ -9093,33 +9206,33 @@
         <v>6.9</v>
       </c>
       <c r="P110" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="Q110" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="R110" t="s">
         <v>44</v>
       </c>
       <c r="S110" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
+        <v>655</v>
+      </c>
+      <c r="B111" t="s">
         <v>656</v>
-      </c>
-      <c r="B111" t="s">
-        <v>657</v>
       </c>
       <c r="C111" s="1" t="n">
         <v>44496</v>
       </c>
       <c r="D111" t="s">
+        <v>657</v>
+      </c>
+      <c r="E111" t="s">
         <v>658</v>
-      </c>
-      <c r="E111" t="s">
-        <v>659</v>
       </c>
       <c r="F111"/>
       <c r="G111" t="n">
@@ -9146,33 +9259,33 @@
       <c r="N111"/>
       <c r="O111"/>
       <c r="P111" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="Q111" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="R111" t="s">
         <v>31</v>
       </c>
       <c r="S111" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
+        <v>661</v>
+      </c>
+      <c r="B112" t="s">
         <v>662</v>
-      </c>
-      <c r="B112" t="s">
-        <v>663</v>
       </c>
       <c r="C112" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D112" t="s">
+        <v>663</v>
+      </c>
+      <c r="E112" t="s">
         <v>664</v>
-      </c>
-      <c r="E112" t="s">
-        <v>665</v>
       </c>
       <c r="F112"/>
       <c r="G112" t="n">
@@ -9192,36 +9305,40 @@
       <c r="M112" t="n">
         <v>3.167</v>
       </c>
-      <c r="N112"/>
-      <c r="O112"/>
+      <c r="N112" t="n">
+        <v>0.1484</v>
+      </c>
+      <c r="O112" t="n">
+        <v>6.7</v>
+      </c>
       <c r="P112" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q112" t="s">
         <v>666</v>
-      </c>
-      <c r="Q112" t="s">
-        <v>667</v>
       </c>
       <c r="R112" t="s">
         <v>44</v>
       </c>
       <c r="S112" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
+        <v>668</v>
+      </c>
+      <c r="B113" t="s">
         <v>669</v>
-      </c>
-      <c r="B113" t="s">
-        <v>670</v>
       </c>
       <c r="C113" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D113" t="s">
+        <v>670</v>
+      </c>
+      <c r="E113" t="s">
         <v>671</v>
-      </c>
-      <c r="E113" t="s">
-        <v>672</v>
       </c>
       <c r="F113"/>
       <c r="G113" t="n">
@@ -9248,83 +9365,83 @@
         <v>21.8</v>
       </c>
       <c r="P113" t="s">
+        <v>671</v>
+      </c>
+      <c r="Q113" t="s">
         <v>672</v>
-      </c>
-      <c r="Q113" t="s">
-        <v>673</v>
       </c>
       <c r="R113" t="s">
         <v>44</v>
       </c>
       <c r="S113" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
+        <v>674</v>
+      </c>
+      <c r="B114" t="s">
         <v>675</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" s="1" t="n">
+        <v>44581</v>
+      </c>
+      <c r="D114" t="s">
         <v>676</v>
       </c>
-      <c r="C114" s="1" t="n">
-        <v>44578</v>
-      </c>
-      <c r="D114" t="s">
+      <c r="E114" t="s">
         <v>677</v>
-      </c>
-      <c r="E114" t="s">
-        <v>678</v>
       </c>
       <c r="F114"/>
       <c r="G114" t="n">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="H114" t="n">
-        <v>4311847</v>
+        <v>4352879</v>
       </c>
       <c r="I114" t="n">
-        <v>324.772</v>
+        <v>327.863</v>
       </c>
       <c r="J114" t="n">
-        <v>17143</v>
+        <v>12585</v>
       </c>
       <c r="K114" t="n">
-        <v>1.291</v>
+        <v>0.948</v>
       </c>
       <c r="L114" t="n">
-        <v>18765</v>
+        <v>15912</v>
       </c>
       <c r="M114" t="n">
-        <v>1.413</v>
+        <v>1.199</v>
       </c>
       <c r="N114"/>
       <c r="O114"/>
       <c r="P114" t="s">
+        <v>677</v>
+      </c>
+      <c r="Q114" t="s">
         <v>678</v>
-      </c>
-      <c r="Q114" t="s">
-        <v>679</v>
       </c>
       <c r="R114" t="s">
         <v>114</v>
       </c>
       <c r="S114" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
+        <v>680</v>
+      </c>
+      <c r="B115" t="s">
         <v>681</v>
-      </c>
-      <c r="B115" t="s">
-        <v>682</v>
       </c>
       <c r="C115" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D115" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E115" t="s">
         <v>36</v>
@@ -9347,36 +9464,40 @@
       <c r="M115" t="n">
         <v>3.53</v>
       </c>
-      <c r="N115"/>
-      <c r="O115"/>
+      <c r="N115" t="n">
+        <v>0.5684</v>
+      </c>
+      <c r="O115" t="n">
+        <v>1.8</v>
+      </c>
       <c r="P115" t="s">
         <v>36</v>
       </c>
       <c r="Q115" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="R115" t="s">
         <v>275</v>
       </c>
       <c r="S115" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
+        <v>685</v>
+      </c>
+      <c r="B116" t="s">
         <v>686</v>
-      </c>
-      <c r="B116" t="s">
-        <v>687</v>
       </c>
       <c r="C116" s="1" t="n">
         <v>44558</v>
       </c>
       <c r="D116" t="s">
+        <v>687</v>
+      </c>
+      <c r="E116" t="s">
         <v>688</v>
-      </c>
-      <c r="E116" t="s">
-        <v>689</v>
       </c>
       <c r="F116"/>
       <c r="G116" t="n">
@@ -9403,30 +9524,30 @@
         <v>7.9</v>
       </c>
       <c r="P116" t="s">
+        <v>688</v>
+      </c>
+      <c r="Q116" t="s">
         <v>689</v>
-      </c>
-      <c r="Q116" t="s">
-        <v>690</v>
       </c>
       <c r="R116" t="s">
         <v>24</v>
       </c>
       <c r="S116" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
+        <v>691</v>
+      </c>
+      <c r="B117" t="s">
         <v>692</v>
-      </c>
-      <c r="B117" t="s">
-        <v>693</v>
       </c>
       <c r="C117" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D117" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E117" t="s">
         <v>36</v>
@@ -9463,30 +9584,30 @@
         <v>36</v>
       </c>
       <c r="Q117" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="R117" t="s">
         <v>44</v>
       </c>
       <c r="S117" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
+        <v>695</v>
+      </c>
+      <c r="B118" t="s">
         <v>696</v>
-      </c>
-      <c r="B118" t="s">
-        <v>697</v>
       </c>
       <c r="C118" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D118" t="s">
+        <v>697</v>
+      </c>
+      <c r="E118" t="s">
         <v>698</v>
-      </c>
-      <c r="E118" t="s">
-        <v>699</v>
       </c>
       <c r="F118"/>
       <c r="G118" t="n">
@@ -9510,39 +9631,43 @@
       <c r="M118" t="n">
         <v>0.123</v>
       </c>
-      <c r="N118"/>
-      <c r="O118"/>
+      <c r="N118" t="n">
+        <v>0.2177</v>
+      </c>
+      <c r="O118" t="n">
+        <v>4.6</v>
+      </c>
       <c r="P118" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="Q118" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="R118" t="s">
         <v>44</v>
       </c>
       <c r="S118" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
+        <v>700</v>
+      </c>
+      <c r="B119" t="s">
         <v>701</v>
-      </c>
-      <c r="B119" t="s">
-        <v>702</v>
       </c>
       <c r="C119" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D119" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E119" t="s">
         <v>36</v>
       </c>
       <c r="F119" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="G119" t="n">
         <v>691</v>
@@ -9565,86 +9690,90 @@
       <c r="M119" t="n">
         <v>4.562</v>
       </c>
-      <c r="N119"/>
-      <c r="O119"/>
+      <c r="N119" t="n">
+        <v>0.4086</v>
+      </c>
+      <c r="O119" t="n">
+        <v>2.4</v>
+      </c>
       <c r="P119" t="s">
         <v>36</v>
       </c>
       <c r="Q119" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="R119" t="s">
         <v>31</v>
       </c>
       <c r="S119" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
+        <v>706</v>
+      </c>
+      <c r="B120" t="s">
         <v>707</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" s="1" t="n">
+        <v>44578</v>
+      </c>
+      <c r="D120" t="s">
         <v>708</v>
-      </c>
-      <c r="C120" s="1" t="n">
-        <v>44571</v>
-      </c>
-      <c r="D120" t="s">
-        <v>709</v>
       </c>
       <c r="E120" t="s">
         <v>36</v>
       </c>
       <c r="F120"/>
       <c r="G120" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H120" t="n">
-        <v>22408065</v>
+        <v>22536079</v>
       </c>
       <c r="I120" t="n">
-        <v>4108.857</v>
+        <v>4132.331</v>
       </c>
       <c r="J120"/>
       <c r="K120"/>
       <c r="L120" t="n">
-        <v>21933</v>
+        <v>18288</v>
       </c>
       <c r="M120" t="n">
-        <v>4.022</v>
+        <v>3.353</v>
       </c>
       <c r="N120" t="n">
-        <v>0.0368</v>
+        <v>0.0517</v>
       </c>
       <c r="O120" t="n">
-        <v>27.2</v>
+        <v>19.3</v>
       </c>
       <c r="P120" t="s">
         <v>36</v>
       </c>
       <c r="Q120" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="R120" t="s">
         <v>114</v>
       </c>
       <c r="S120" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
+        <v>711</v>
+      </c>
+      <c r="B121" t="s">
         <v>712</v>
-      </c>
-      <c r="B121" t="s">
-        <v>713</v>
       </c>
       <c r="C121" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D121" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E121" t="s">
         <v>36</v>
@@ -9681,30 +9810,30 @@
         <v>36</v>
       </c>
       <c r="Q121" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="R121" t="s">
         <v>44</v>
       </c>
       <c r="S121" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
+        <v>715</v>
+      </c>
+      <c r="B122" t="s">
         <v>716</v>
-      </c>
-      <c r="B122" t="s">
-        <v>717</v>
       </c>
       <c r="C122" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D122" t="s">
+        <v>717</v>
+      </c>
+      <c r="E122" t="s">
         <v>718</v>
-      </c>
-      <c r="E122" t="s">
-        <v>719</v>
       </c>
       <c r="F122"/>
       <c r="G122" t="n">
@@ -9735,148 +9864,148 @@
         <v>1.9</v>
       </c>
       <c r="P122" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="Q122" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="R122" t="s">
         <v>44</v>
       </c>
       <c r="S122" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
+        <v>720</v>
+      </c>
+      <c r="B123" t="s">
         <v>721</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" s="1" t="n">
+        <v>44578</v>
+      </c>
+      <c r="D123" t="s">
         <v>722</v>
       </c>
-      <c r="C123" s="1" t="n">
-        <v>44576</v>
-      </c>
-      <c r="D123" t="s">
+      <c r="E123" t="s">
         <v>723</v>
       </c>
-      <c r="E123" t="s">
+      <c r="F123" t="s">
         <v>724</v>
       </c>
-      <c r="F123" t="s">
+      <c r="G123" t="n">
+        <v>677</v>
+      </c>
+      <c r="H123" t="n">
+        <v>21815463</v>
+      </c>
+      <c r="I123" t="n">
+        <v>363.337</v>
+      </c>
+      <c r="J123" t="n">
+        <v>18171</v>
+      </c>
+      <c r="K123" t="n">
+        <v>0.303</v>
+      </c>
+      <c r="L123" t="n">
+        <v>34986</v>
+      </c>
+      <c r="M123" t="n">
+        <v>0.583</v>
+      </c>
+      <c r="N123" t="n">
+        <v>0.1325</v>
+      </c>
+      <c r="O123" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="P123" t="s">
         <v>725</v>
       </c>
-      <c r="G123" t="n">
-        <v>675</v>
-      </c>
-      <c r="H123" t="n">
-        <v>21772893</v>
-      </c>
-      <c r="I123" t="n">
-        <v>362.628</v>
-      </c>
-      <c r="J123" t="n">
-        <v>36593</v>
-      </c>
-      <c r="K123" t="n">
-        <v>0.609</v>
-      </c>
-      <c r="L123" t="n">
-        <v>36098</v>
-      </c>
-      <c r="M123" t="n">
-        <v>0.601</v>
-      </c>
-      <c r="N123" t="n">
-        <v>0.1388</v>
-      </c>
-      <c r="O123" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="P123" t="s">
-        <v>726</v>
-      </c>
       <c r="Q123" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="R123" t="s">
         <v>31</v>
       </c>
       <c r="S123" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
+        <v>727</v>
+      </c>
+      <c r="B124" t="s">
         <v>728</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" s="1" t="n">
+        <v>44578</v>
+      </c>
+      <c r="D124" t="s">
         <v>729</v>
       </c>
-      <c r="C124" s="1" t="n">
-        <v>44571</v>
-      </c>
-      <c r="D124" t="s">
+      <c r="E124" t="s">
         <v>730</v>
       </c>
-      <c r="E124" t="s">
+      <c r="F124" t="s">
         <v>731</v>
       </c>
-      <c r="F124" t="s">
+      <c r="G124" t="n">
+        <v>710</v>
+      </c>
+      <c r="H124" t="n">
+        <v>48410361</v>
+      </c>
+      <c r="I124" t="n">
+        <v>943.576</v>
+      </c>
+      <c r="J124" t="n">
+        <v>123144</v>
+      </c>
+      <c r="K124" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="L124" t="n">
+        <v>171494</v>
+      </c>
+      <c r="M124" t="n">
+        <v>3.343</v>
+      </c>
+      <c r="N124" t="n">
+        <v>0.0247</v>
+      </c>
+      <c r="O124" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="P124" t="s">
         <v>732</v>
       </c>
-      <c r="G124" t="n">
-        <v>703</v>
-      </c>
-      <c r="H124" t="n">
-        <v>47302915</v>
-      </c>
-      <c r="I124" t="n">
-        <v>921.991</v>
-      </c>
-      <c r="J124" t="n">
-        <v>48606</v>
-      </c>
-      <c r="K124" t="n">
-        <v>0.947</v>
-      </c>
-      <c r="L124" t="n">
-        <v>193966</v>
-      </c>
-      <c r="M124" t="n">
-        <v>3.781</v>
-      </c>
-      <c r="N124" t="n">
-        <v>0.0186</v>
-      </c>
-      <c r="O124" t="n">
-        <v>53.8</v>
-      </c>
-      <c r="P124" t="s">
+      <c r="Q124" t="s">
         <v>733</v>
-      </c>
-      <c r="Q124" t="s">
-        <v>734</v>
       </c>
       <c r="R124" t="s">
         <v>31</v>
       </c>
       <c r="S124" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
+        <v>735</v>
+      </c>
+      <c r="B125" t="s">
         <v>736</v>
-      </c>
-      <c r="B125" t="s">
-        <v>737</v>
       </c>
       <c r="C125" s="1" t="n">
         <v>44342</v>
       </c>
       <c r="D125" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E125" t="s">
         <v>36</v>
@@ -9909,30 +10038,30 @@
         <v>36</v>
       </c>
       <c r="Q125" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="R125" t="s">
         <v>44</v>
       </c>
       <c r="S125" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
+        <v>740</v>
+      </c>
+      <c r="B126" t="s">
         <v>741</v>
-      </c>
-      <c r="B126" t="s">
-        <v>742</v>
       </c>
       <c r="C126" s="1" t="n">
         <v>44574</v>
       </c>
       <c r="D126" t="s">
+        <v>742</v>
+      </c>
+      <c r="E126" t="s">
         <v>743</v>
-      </c>
-      <c r="E126" t="s">
-        <v>744</v>
       </c>
       <c r="F126"/>
       <c r="G126" t="n">
@@ -9959,33 +10088,33 @@
         <v>2.4</v>
       </c>
       <c r="P126" t="s">
+        <v>744</v>
+      </c>
+      <c r="Q126" t="s">
         <v>745</v>
-      </c>
-      <c r="Q126" t="s">
-        <v>746</v>
       </c>
       <c r="R126" t="s">
         <v>44</v>
       </c>
       <c r="S126" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
+        <v>747</v>
+      </c>
+      <c r="B127" t="s">
         <v>748</v>
-      </c>
-      <c r="B127" t="s">
-        <v>749</v>
       </c>
       <c r="C127" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D127" t="s">
+        <v>749</v>
+      </c>
+      <c r="E127" t="s">
         <v>750</v>
-      </c>
-      <c r="E127" t="s">
-        <v>751</v>
       </c>
       <c r="F127"/>
       <c r="G127" t="n">
@@ -10009,36 +10138,40 @@
       <c r="M127" t="n">
         <v>0.335</v>
       </c>
-      <c r="N127"/>
-      <c r="O127"/>
+      <c r="N127" t="n">
+        <v>0.0973</v>
+      </c>
+      <c r="O127" t="n">
+        <v>10.3</v>
+      </c>
       <c r="P127" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="Q127" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="R127" t="s">
         <v>44</v>
       </c>
       <c r="S127" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
+        <v>752</v>
+      </c>
+      <c r="B128" t="s">
         <v>753</v>
-      </c>
-      <c r="B128" t="s">
-        <v>754</v>
       </c>
       <c r="C128" s="1" t="n">
         <v>44556</v>
       </c>
       <c r="D128" t="s">
+        <v>754</v>
+      </c>
+      <c r="E128" t="s">
         <v>755</v>
-      </c>
-      <c r="E128" t="s">
-        <v>756</v>
       </c>
       <c r="F128"/>
       <c r="G128" t="n">
@@ -10065,33 +10198,33 @@
         <v>15.5</v>
       </c>
       <c r="P128" t="s">
+        <v>756</v>
+      </c>
+      <c r="Q128" t="s">
         <v>757</v>
-      </c>
-      <c r="Q128" t="s">
-        <v>758</v>
       </c>
       <c r="R128" t="s">
         <v>44</v>
       </c>
       <c r="S128" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
+        <v>759</v>
+      </c>
+      <c r="B129" t="s">
         <v>760</v>
-      </c>
-      <c r="B129" t="s">
-        <v>761</v>
       </c>
       <c r="C129" s="1" t="n">
         <v>44576</v>
       </c>
       <c r="D129" t="s">
+        <v>472</v>
+      </c>
+      <c r="E129" t="s">
         <v>473</v>
-      </c>
-      <c r="E129" t="s">
-        <v>474</v>
       </c>
       <c r="F129"/>
       <c r="G129" t="n">
@@ -10122,33 +10255,33 @@
         <v>2.8</v>
       </c>
       <c r="P129" t="s">
+        <v>473</v>
+      </c>
+      <c r="Q129" t="s">
         <v>474</v>
-      </c>
-      <c r="Q129" t="s">
-        <v>475</v>
       </c>
       <c r="R129" t="s">
         <v>44</v>
       </c>
       <c r="S129" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
+        <v>762</v>
+      </c>
+      <c r="B130" t="s">
         <v>763</v>
-      </c>
-      <c r="B130" t="s">
-        <v>764</v>
       </c>
       <c r="C130" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D130" t="s">
+        <v>764</v>
+      </c>
+      <c r="E130" t="s">
         <v>765</v>
-      </c>
-      <c r="E130" t="s">
-        <v>766</v>
       </c>
       <c r="F130"/>
       <c r="G130" t="n">
@@ -10172,36 +10305,40 @@
       <c r="M130" t="n">
         <v>0.934</v>
       </c>
-      <c r="N130"/>
-      <c r="O130"/>
+      <c r="N130" t="n">
+        <v>0.0031</v>
+      </c>
+      <c r="O130" t="n">
+        <v>317.6</v>
+      </c>
       <c r="P130" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="Q130" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="R130" t="s">
         <v>31</v>
       </c>
       <c r="S130" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
+        <v>767</v>
+      </c>
+      <c r="B131" t="s">
         <v>768</v>
-      </c>
-      <c r="B131" t="s">
-        <v>769</v>
       </c>
       <c r="C131" s="1" t="n">
         <v>44576</v>
       </c>
       <c r="D131" t="s">
+        <v>769</v>
+      </c>
+      <c r="E131" t="s">
         <v>770</v>
-      </c>
-      <c r="E131" t="s">
-        <v>771</v>
       </c>
       <c r="F131"/>
       <c r="G131" t="n">
@@ -10225,33 +10362,37 @@
       <c r="M131" t="n">
         <v>0.903</v>
       </c>
-      <c r="N131"/>
-      <c r="O131"/>
+      <c r="N131" t="n">
+        <v>0.1076</v>
+      </c>
+      <c r="O131" t="n">
+        <v>9.3</v>
+      </c>
       <c r="P131" t="s">
+        <v>771</v>
+      </c>
+      <c r="Q131" t="s">
         <v>772</v>
-      </c>
-      <c r="Q131" t="s">
-        <v>773</v>
       </c>
       <c r="R131" t="s">
         <v>44</v>
       </c>
       <c r="S131" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
+        <v>774</v>
+      </c>
+      <c r="B132" t="s">
         <v>775</v>
-      </c>
-      <c r="B132" t="s">
-        <v>776</v>
       </c>
       <c r="C132" s="1" t="n">
         <v>44489</v>
       </c>
       <c r="D132" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E132" t="s">
         <v>36</v>
@@ -10284,31 +10425,31 @@
         <v>36</v>
       </c>
       <c r="Q132" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="R132" t="s">
         <v>24</v>
       </c>
       <c r="S132" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
+        <v>778</v>
+      </c>
+      <c r="B133" t="s">
         <v>779</v>
-      </c>
-      <c r="B133" t="s">
-        <v>780</v>
       </c>
       <c r="C133" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D133"/>
       <c r="E133" t="s">
+        <v>780</v>
+      </c>
+      <c r="F133" t="s">
         <v>781</v>
-      </c>
-      <c r="F133" t="s">
-        <v>782</v>
       </c>
       <c r="G133" t="n">
         <v>678</v>
@@ -10338,30 +10479,30 @@
         <v>6.5</v>
       </c>
       <c r="P133" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="Q133" t="s">
+        <v>782</v>
+      </c>
+      <c r="R133" t="s">
         <v>783</v>
       </c>
-      <c r="R133" t="s">
+      <c r="S133" t="s">
         <v>784</v>
-      </c>
-      <c r="S133" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
+        <v>785</v>
+      </c>
+      <c r="B134" t="s">
         <v>786</v>
-      </c>
-      <c r="B134" t="s">
-        <v>787</v>
       </c>
       <c r="C134" s="1" t="n">
         <v>44475</v>
       </c>
       <c r="D134" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E134" t="s">
         <v>36</v>
@@ -10398,30 +10539,30 @@
         <v>36</v>
       </c>
       <c r="Q134" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="R134" t="s">
         <v>31</v>
       </c>
       <c r="S134" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
+        <v>790</v>
+      </c>
+      <c r="B135" t="s">
         <v>791</v>
-      </c>
-      <c r="B135" t="s">
-        <v>792</v>
       </c>
       <c r="C135" s="1" t="n">
         <v>44576</v>
       </c>
       <c r="D135" t="s">
+        <v>792</v>
+      </c>
+      <c r="E135" t="s">
         <v>793</v>
-      </c>
-      <c r="E135" t="s">
-        <v>794</v>
       </c>
       <c r="F135"/>
       <c r="G135" t="n">
@@ -10448,33 +10589,33 @@
         <v>4.3</v>
       </c>
       <c r="P135" t="s">
+        <v>794</v>
+      </c>
+      <c r="Q135" t="s">
         <v>795</v>
-      </c>
-      <c r="Q135" t="s">
-        <v>796</v>
       </c>
       <c r="R135" t="s">
         <v>31</v>
       </c>
       <c r="S135" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
+        <v>797</v>
+      </c>
+      <c r="B136" t="s">
         <v>798</v>
-      </c>
-      <c r="B136" t="s">
-        <v>799</v>
       </c>
       <c r="C136" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D136" t="s">
+        <v>799</v>
+      </c>
+      <c r="E136" t="s">
         <v>800</v>
-      </c>
-      <c r="E136" t="s">
-        <v>801</v>
       </c>
       <c r="F136"/>
       <c r="G136" t="n">
@@ -10505,33 +10646,33 @@
         <v>5.9</v>
       </c>
       <c r="P136" t="s">
+        <v>800</v>
+      </c>
+      <c r="Q136" t="s">
         <v>801</v>
-      </c>
-      <c r="Q136" t="s">
-        <v>802</v>
       </c>
       <c r="R136" t="s">
         <v>44</v>
       </c>
       <c r="S136" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
+        <v>803</v>
+      </c>
+      <c r="B137" t="s">
         <v>804</v>
-      </c>
-      <c r="B137" t="s">
-        <v>805</v>
       </c>
       <c r="C137" s="1" t="n">
         <v>44576</v>
       </c>
       <c r="D137" t="s">
+        <v>805</v>
+      </c>
+      <c r="E137" t="s">
         <v>806</v>
-      </c>
-      <c r="E137" t="s">
-        <v>807</v>
       </c>
       <c r="F137"/>
       <c r="G137" t="n">
@@ -10562,86 +10703,86 @@
         <v>10.2</v>
       </c>
       <c r="P137" t="s">
+        <v>806</v>
+      </c>
+      <c r="Q137" t="s">
         <v>807</v>
-      </c>
-      <c r="Q137" t="s">
-        <v>808</v>
       </c>
       <c r="R137" t="s">
         <v>114</v>
       </c>
       <c r="S137" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
+        <v>809</v>
+      </c>
+      <c r="B138" t="s">
         <v>810</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" s="1" t="n">
+        <v>44581</v>
+      </c>
+      <c r="D138" t="s">
         <v>811</v>
       </c>
-      <c r="C138" s="1" t="n">
-        <v>44578</v>
-      </c>
-      <c r="D138" t="s">
+      <c r="E138" t="s">
         <v>812</v>
-      </c>
-      <c r="E138" t="s">
-        <v>813</v>
       </c>
       <c r="F138"/>
       <c r="G138" t="n">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="H138" t="n">
-        <v>17182817</v>
+        <v>17332435</v>
       </c>
       <c r="I138" t="n">
-        <v>395.309</v>
+        <v>398.751</v>
       </c>
       <c r="J138" t="n">
-        <v>14616</v>
+        <v>61642</v>
       </c>
       <c r="K138" t="n">
-        <v>0.336</v>
+        <v>1.418</v>
       </c>
       <c r="L138" t="n">
-        <v>30853</v>
+        <v>37281</v>
       </c>
       <c r="M138" t="n">
-        <v>0.71</v>
+        <v>0.858</v>
       </c>
       <c r="N138"/>
       <c r="O138"/>
       <c r="P138" t="s">
+        <v>812</v>
+      </c>
+      <c r="Q138" t="s">
         <v>813</v>
-      </c>
-      <c r="Q138" t="s">
-        <v>814</v>
       </c>
       <c r="R138" t="s">
         <v>44</v>
       </c>
       <c r="S138" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
+        <v>815</v>
+      </c>
+      <c r="B139" t="s">
         <v>816</v>
-      </c>
-      <c r="B139" t="s">
-        <v>817</v>
       </c>
       <c r="C139" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D139" t="s">
+        <v>817</v>
+      </c>
+      <c r="E139" t="s">
         <v>818</v>
-      </c>
-      <c r="E139" t="s">
-        <v>819</v>
       </c>
       <c r="F139"/>
       <c r="G139" t="n">
@@ -10665,36 +10806,40 @@
       <c r="M139" t="n">
         <v>35.302</v>
       </c>
-      <c r="N139"/>
-      <c r="O139"/>
+      <c r="N139" t="n">
+        <v>0.0081</v>
+      </c>
+      <c r="O139" t="n">
+        <v>123.1</v>
+      </c>
       <c r="P139" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="Q139" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="R139" t="s">
         <v>44</v>
       </c>
       <c r="S139" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
+        <v>820</v>
+      </c>
+      <c r="B140" t="s">
         <v>821</v>
-      </c>
-      <c r="B140" t="s">
-        <v>822</v>
       </c>
       <c r="C140" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D140" t="s">
+        <v>822</v>
+      </c>
+      <c r="E140" t="s">
         <v>823</v>
-      </c>
-      <c r="E140" t="s">
-        <v>824</v>
       </c>
       <c r="F140"/>
       <c r="G140" t="n">
@@ -10725,87 +10870,87 @@
         <v>13.7</v>
       </c>
       <c r="P140" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q140" t="s">
         <v>825</v>
-      </c>
-      <c r="Q140" t="s">
-        <v>826</v>
       </c>
       <c r="R140" t="s">
         <v>44</v>
       </c>
       <c r="S140" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
+        <v>827</v>
+      </c>
+      <c r="B141" t="s">
         <v>828</v>
       </c>
-      <c r="B141" t="s">
+      <c r="C141" s="1" t="n">
+        <v>44575</v>
+      </c>
+      <c r="D141" t="s">
         <v>829</v>
       </c>
-      <c r="C141" s="1" t="n">
-        <v>44572</v>
-      </c>
-      <c r="D141" t="s">
+      <c r="E141" t="s">
         <v>830</v>
-      </c>
-      <c r="E141" t="s">
-        <v>831</v>
       </c>
       <c r="F141"/>
       <c r="G141" t="n">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="H141" t="n">
-        <v>747501153</v>
+        <v>751696571</v>
       </c>
       <c r="I141" t="n">
-        <v>2245.321</v>
+        <v>2257.923</v>
       </c>
       <c r="J141" t="n">
-        <v>2157306</v>
+        <v>780237</v>
       </c>
       <c r="K141" t="n">
-        <v>6.48</v>
+        <v>2.344</v>
       </c>
       <c r="L141" t="n">
-        <v>2331399</v>
+        <v>1682636</v>
       </c>
       <c r="M141" t="n">
-        <v>7.003</v>
+        <v>5.054</v>
       </c>
       <c r="N141" t="n">
-        <v>0.3238</v>
+        <v>0.4678</v>
       </c>
       <c r="O141" t="n">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="P141" t="s">
+        <v>830</v>
+      </c>
+      <c r="Q141" t="s">
+        <v>829</v>
+      </c>
+      <c r="R141" t="s">
         <v>831</v>
       </c>
-      <c r="Q141" t="s">
-        <v>830</v>
-      </c>
-      <c r="R141" t="s">
+      <c r="S141" t="s">
         <v>832</v>
-      </c>
-      <c r="S141" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
+        <v>833</v>
+      </c>
+      <c r="B142" t="s">
         <v>834</v>
-      </c>
-      <c r="B142" t="s">
-        <v>835</v>
       </c>
       <c r="C142" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D142" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E142" t="s">
         <v>205</v>
@@ -10842,30 +10987,30 @@
         <v>205</v>
       </c>
       <c r="Q142" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="R142" t="s">
         <v>44</v>
       </c>
       <c r="S142" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
+        <v>837</v>
+      </c>
+      <c r="B143" t="s">
         <v>838</v>
-      </c>
-      <c r="B143" t="s">
-        <v>839</v>
       </c>
       <c r="C143" s="1" t="n">
         <v>44575</v>
       </c>
       <c r="D143" t="s">
+        <v>839</v>
+      </c>
+      <c r="E143" t="s">
         <v>840</v>
-      </c>
-      <c r="E143" t="s">
-        <v>841</v>
       </c>
       <c r="F143"/>
       <c r="G143" t="n">
@@ -10892,33 +11037,33 @@
         <v>4.4</v>
       </c>
       <c r="P143" t="s">
+        <v>841</v>
+      </c>
+      <c r="Q143" t="s">
         <v>842</v>
-      </c>
-      <c r="Q143" t="s">
-        <v>843</v>
       </c>
       <c r="R143" t="s">
         <v>114</v>
       </c>
       <c r="S143" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
+        <v>844</v>
+      </c>
+      <c r="B144" t="s">
         <v>845</v>
-      </c>
-      <c r="B144" t="s">
-        <v>846</v>
       </c>
       <c r="C144" s="1" t="n">
         <v>44578</v>
       </c>
       <c r="D144" t="s">
+        <v>846</v>
+      </c>
+      <c r="E144" t="s">
         <v>847</v>
-      </c>
-      <c r="E144" t="s">
-        <v>848</v>
       </c>
       <c r="F144"/>
       <c r="G144" t="n">
@@ -10942,36 +11087,40 @@
       <c r="M144" t="n">
         <v>0.413</v>
       </c>
-      <c r="N144"/>
-      <c r="O144"/>
+      <c r="N144" t="n">
+        <v>0.227</v>
+      </c>
+      <c r="O144" t="n">
+        <v>4.4</v>
+      </c>
       <c r="P144" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="Q144" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="R144" t="s">
         <v>44</v>
       </c>
       <c r="S144" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
+        <v>850</v>
+      </c>
+      <c r="B145" t="s">
         <v>851</v>
-      </c>
-      <c r="B145" t="s">
-        <v>852</v>
       </c>
       <c r="C145" s="1" t="n">
         <v>44577</v>
       </c>
       <c r="D145" t="s">
+        <v>852</v>
+      </c>
+      <c r="E145" t="s">
         <v>853</v>
-      </c>
-      <c r="E145" t="s">
-        <v>854</v>
       </c>
       <c r="F145"/>
       <c r="G145" t="n">
@@ -11002,16 +11151,16 @@
         <v>9.7</v>
       </c>
       <c r="P145" t="s">
+        <v>853</v>
+      </c>
+      <c r="Q145" t="s">
         <v>854</v>
-      </c>
-      <c r="Q145" t="s">
-        <v>855</v>
       </c>
       <c r="R145" t="s">
         <v>44</v>
       </c>
       <c r="S145" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
   </sheetData>

</xml_diff>